<commit_message>
mpc working with n_horizon 50
</commit_message>
<xml_diff>
--- a/Tests/mpc tests.xlsx
+++ b/Tests/mpc tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\Documents\FYP\pyLanderSim\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587DAC3-26BC-4D31-A484-CD487ECD030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FE5EDA-DFED-4621-8651-2C0000F5C787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6432363C-8F0D-466E-8FFF-1F4EB92E218D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Base case</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>TVC Lander Testing</t>
+  </si>
+  <si>
+    <t>lterm = (r_x - x)**2 + (r_z - z)**2 + (r_dx - dx)**2 + (r_dz - dz)**2</t>
+  </si>
+  <si>
+    <t>n_horizon = 50</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$17</c:f>
+              <c:f>Sheet1!$A$9:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -269,15 +275,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$17</c:f>
+              <c:f>Sheet1!$B$9:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>13.47</c:v>
+                  <c:v>-0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.58</c:v>
+                  <c:v>-3.5638046534758501E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>13.62</c:v>
@@ -289,7 +295,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.37</c:v>
+                  <c:v>-0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>13.19</c:v>
@@ -304,7 +310,7 @@
                   <c:v>12.56</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.31</c:v>
+                  <c:v>-0.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -607,7 +613,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$60:$A$70</c:f>
+              <c:f>Sheet1!$A$62:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -649,7 +655,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$60:$C$70</c:f>
+              <c:f>Sheet1!$C$62:$C$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -987,7 +993,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$73:$A$83</c:f>
+              <c:f>Sheet1!$A$75:$A$85</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1029,7 +1035,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$73:$B$83</c:f>
+              <c:f>Sheet1!$B$75:$B$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1367,7 +1373,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$73:$A$83</c:f>
+              <c:f>Sheet1!$A$75:$A$85</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1409,7 +1415,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$73:$C$83</c:f>
+              <c:f>Sheet1!$C$75:$C$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1755,7 +1761,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$87:$A$97</c:f>
+              <c:f>Sheet1!$A$89:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1797,7 +1803,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$87:$B$97</c:f>
+              <c:f>Sheet1!$B$89:$B$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2135,7 +2141,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$87:$A$97</c:f>
+              <c:f>Sheet1!$A$89:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2177,7 +2183,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$87:$C$97</c:f>
+              <c:f>Sheet1!$C$89:$C$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2523,7 +2529,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$100:$A$110</c:f>
+              <c:f>Sheet1!$A$102:$A$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2565,7 +2571,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$100:$B$110</c:f>
+              <c:f>Sheet1!$B$102:$B$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2903,7 +2909,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$100:$A$110</c:f>
+              <c:f>Sheet1!$A$102:$A$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2945,7 +2951,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$100:$C$110</c:f>
+              <c:f>Sheet1!$C$102:$C$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3283,7 +3289,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$17</c:f>
+              <c:f>Sheet1!$A$9:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3325,15 +3331,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$17</c:f>
+              <c:f>Sheet1!$C$9:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>116.89</c:v>
+                  <c:v>111.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.89</c:v>
+                  <c:v>113.032300863378</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>118.99</c:v>
@@ -3345,7 +3351,7 @@
                   <c:v>121.58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>127.58</c:v>
+                  <c:v>117.61</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>124.95</c:v>
@@ -3360,7 +3366,7 @@
                   <c:v>133.08000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>137.94</c:v>
+                  <c:v>123.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3663,7 +3669,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$20:$A$30</c:f>
+              <c:f>Sheet1!$A$22:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3705,7 +3711,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$B$30</c:f>
+              <c:f>Sheet1!$B$22:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4043,7 +4049,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$20:$A$30</c:f>
+              <c:f>Sheet1!$A$22:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4085,7 +4091,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$30</c:f>
+              <c:f>Sheet1!$C$22:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4423,7 +4429,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$43</c:f>
+              <c:f>Sheet1!$A$35:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4465,7 +4471,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$B$43</c:f>
+              <c:f>Sheet1!$B$35:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4803,7 +4809,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$43</c:f>
+              <c:f>Sheet1!$A$35:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4845,7 +4851,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$33:$C$43</c:f>
+              <c:f>Sheet1!$C$35:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5183,7 +5189,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$46:$A$56</c:f>
+              <c:f>Sheet1!$A$48:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5225,7 +5231,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$46:$B$56</c:f>
+              <c:f>Sheet1!$B$48:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5563,7 +5569,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$46:$A$56</c:f>
+              <c:f>Sheet1!$A$48:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5605,7 +5611,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$46:$C$56</c:f>
+              <c:f>Sheet1!$C$48:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5943,7 +5949,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$60:$A$70</c:f>
+              <c:f>Sheet1!$A$62:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5985,7 +5991,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$60:$B$70</c:f>
+              <c:f>Sheet1!$B$62:$B$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -16021,10 +16027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53024B73-4110-4BB0-AABF-5DA1AF3A9961}">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16040,189 +16046,177 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>-0.37</v>
-      </c>
-      <c r="C4">
-        <v>127.58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="B7">
-        <v>13.47</v>
-      </c>
-      <c r="C7">
-        <v>116.89</v>
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>-0.04</v>
+      </c>
+      <c r="C6">
+        <v>117.61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>0.96</v>
-      </c>
-      <c r="B8">
-        <v>13.58</v>
-      </c>
-      <c r="C8">
-        <v>117.89</v>
+      <c r="A8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="B9">
-        <v>13.62</v>
+        <v>-0.04</v>
       </c>
       <c r="C9">
-        <v>118.99</v>
+        <v>111.92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="B10">
-        <v>13.59</v>
+        <v>-3.5638046534758501E-2</v>
       </c>
       <c r="C10">
-        <v>120.21</v>
+        <v>113.032300863378</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="B11">
-        <v>13.5</v>
+        <v>13.62</v>
       </c>
       <c r="C11">
-        <v>121.58</v>
+        <v>118.99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="B12">
-        <f>B4</f>
-        <v>-0.37</v>
+        <v>13.59</v>
       </c>
       <c r="C12">
-        <f>C4</f>
-        <v>127.58</v>
+        <v>120.21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="B13">
-        <v>13.19</v>
+        <v>13.5</v>
       </c>
       <c r="C13">
-        <v>124.95</v>
+        <v>121.58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>13.02</v>
+        <f>B6</f>
+        <v>-0.04</v>
       </c>
       <c r="C14">
-        <v>127.08</v>
+        <f>C6</f>
+        <v>117.61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="B15">
-        <v>12.79</v>
+        <v>13.19</v>
       </c>
       <c r="C15">
-        <v>129.69999999999999</v>
+        <v>124.95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>1.04</v>
+        <v>1.02</v>
       </c>
       <c r="B16">
-        <v>12.56</v>
+        <v>13.02</v>
       </c>
       <c r="C16">
-        <v>133.08000000000001</v>
+        <v>127.08</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="B17">
-        <v>12.31</v>
+        <v>12.79</v>
       </c>
       <c r="C17">
-        <v>137.94</v>
+        <v>129.69999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="B18">
+        <v>12.56</v>
+      </c>
+      <c r="C18">
+        <v>133.08000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="B20">
-        <v>13.9</v>
-      </c>
-      <c r="C20">
-        <v>123.14</v>
+      <c r="A19" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="B19">
+        <v>-0.04</v>
+      </c>
+      <c r="C19">
+        <v>123.38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>0.96</v>
-      </c>
-      <c r="B21">
-        <v>13.77</v>
-      </c>
-      <c r="C21">
-        <v>123.15</v>
+      <c r="A21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="B22">
-        <v>13.68</v>
+        <v>13.9</v>
       </c>
       <c r="C22">
         <v>123.14</v>
@@ -16230,10 +16224,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="B23">
-        <v>13.55</v>
+        <v>13.77</v>
       </c>
       <c r="C23">
         <v>123.15</v>
@@ -16241,10 +16235,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="B24">
-        <v>13.46</v>
+        <v>13.68</v>
       </c>
       <c r="C24">
         <v>123.14</v>
@@ -16252,43 +16246,43 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="B25">
-        <v>13.37</v>
+        <v>13.55</v>
       </c>
       <c r="C25">
-        <v>123.14</v>
+        <v>123.15</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="B26">
-        <v>13.25</v>
+        <v>13.46</v>
       </c>
       <c r="C26">
-        <v>123.15</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="B27">
-        <v>13.16</v>
+        <v>13.37</v>
       </c>
       <c r="C27">
-        <v>123.15</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="B28">
-        <v>13.07</v>
+        <v>13.25</v>
       </c>
       <c r="C28">
         <v>123.15</v>
@@ -16296,10 +16290,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>1.04</v>
+        <v>1.02</v>
       </c>
       <c r="B29">
-        <v>12.94</v>
+        <v>13.16</v>
       </c>
       <c r="C29">
         <v>123.15</v>
@@ -16307,768 +16301,790 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="B30">
-        <v>12.85</v>
+        <v>13.07</v>
       </c>
       <c r="C30">
         <v>123.15</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="B31">
+        <v>12.94</v>
+      </c>
+      <c r="C31">
+        <v>123.15</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B33">
-        <v>12.19</v>
-      </c>
-      <c r="C33">
-        <v>123.78</v>
+      <c r="A32" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="B32">
+        <v>12.85</v>
+      </c>
+      <c r="C32">
+        <v>123.15</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>0.92</v>
-      </c>
-      <c r="B34">
-        <v>12.45</v>
-      </c>
-      <c r="C34">
-        <v>123.58</v>
+      <c r="A34" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="B35">
-        <v>12.68</v>
+        <v>12.19</v>
       </c>
       <c r="C35">
-        <v>123.42</v>
+        <v>123.78</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="B36">
-        <v>12.93</v>
+        <v>12.45</v>
       </c>
       <c r="C36">
-        <v>123.29</v>
+        <v>123.58</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="B37">
-        <v>13.14</v>
+        <v>12.68</v>
       </c>
       <c r="C37">
-        <v>123.2</v>
+        <v>123.42</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="B38">
-        <v>13.37</v>
+        <v>12.93</v>
       </c>
       <c r="C38">
-        <v>123.14</v>
+        <v>123.29</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="B39">
-        <v>13.54</v>
+        <v>13.14</v>
       </c>
       <c r="C39">
-        <v>123.14</v>
+        <v>123.2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="B40">
-        <v>13.73</v>
+        <v>13.37</v>
       </c>
       <c r="C40">
-        <v>123.19</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
       <c r="B41">
-        <v>13.94</v>
+        <v>13.54</v>
       </c>
       <c r="C41">
-        <v>123.27</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>1.08</v>
+        <v>1.04</v>
       </c>
       <c r="B42">
-        <v>14.09</v>
+        <v>13.73</v>
       </c>
       <c r="C42">
-        <v>123.41</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="B43">
-        <v>14.27</v>
+        <v>13.94</v>
       </c>
       <c r="C43">
-        <v>123.6</v>
+        <v>123.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="B44">
+        <v>14.09</v>
+      </c>
+      <c r="C44">
+        <v>123.41</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B46">
-        <v>13.53</v>
-      </c>
-      <c r="C46">
-        <v>123.21</v>
+      <c r="A45" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B45">
+        <v>14.27</v>
+      </c>
+      <c r="C45">
+        <v>123.6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>0.92</v>
-      </c>
-      <c r="B47">
-        <v>13.48</v>
-      </c>
-      <c r="C47">
-        <v>123.2</v>
+      <c r="A47" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="B48">
-        <v>13.44</v>
+        <v>13.53</v>
       </c>
       <c r="C48">
-        <v>123.19</v>
+        <v>123.21</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="B49">
-        <v>13.43</v>
+        <v>13.48</v>
       </c>
       <c r="C49">
-        <v>123.17</v>
+        <v>123.2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="B50">
-        <v>13.38</v>
+        <v>13.44</v>
       </c>
       <c r="C50">
-        <v>123.16</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="B51">
-        <v>13.37</v>
+        <v>13.43</v>
       </c>
       <c r="C51">
-        <v>123.14</v>
+        <v>123.17</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="B52">
-        <v>13.33</v>
+        <v>13.38</v>
       </c>
       <c r="C52">
-        <v>123.13</v>
+        <v>123.16</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="B53">
-        <v>13.28</v>
+        <v>13.37</v>
       </c>
       <c r="C53">
-        <v>123.12</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
       <c r="B54">
-        <v>13.27</v>
+        <v>13.33</v>
       </c>
       <c r="C54">
-        <v>123.1</v>
+        <v>123.13</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>1.08</v>
+        <v>1.04</v>
       </c>
       <c r="B55">
-        <v>13.23</v>
+        <v>13.28</v>
       </c>
       <c r="C55">
-        <v>123.09</v>
+        <v>123.12</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="B56">
+        <v>13.27</v>
+      </c>
+      <c r="C56">
+        <v>123.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="B57">
+        <v>13.23</v>
+      </c>
+      <c r="C57">
+        <v>123.09</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B56">
+      <c r="B58">
         <v>13.22</v>
       </c>
-      <c r="C56">
+      <c r="C58">
         <v>123.08</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B60">
-        <v>13.79</v>
-      </c>
-      <c r="C60">
-        <v>121.09</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>0.92</v>
-      </c>
-      <c r="B61">
-        <v>13.7</v>
-      </c>
-      <c r="C61">
-        <v>121.35</v>
+      <c r="A61" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="B62">
-        <v>13.6</v>
+        <v>13.79</v>
       </c>
       <c r="C62">
-        <v>121.69</v>
+        <v>121.09</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="B63">
-        <v>13.54</v>
+        <v>13.7</v>
       </c>
       <c r="C63">
-        <v>122.11</v>
+        <v>121.35</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="B64">
-        <v>13.44</v>
+        <v>13.6</v>
       </c>
       <c r="C64">
-        <v>122.6</v>
+        <v>121.69</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="B65">
-        <v>13.37</v>
+        <v>13.54</v>
       </c>
       <c r="C65">
-        <v>123.14</v>
+        <v>122.11</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="B66">
-        <v>13.26</v>
+        <v>13.44</v>
       </c>
       <c r="C66">
-        <v>123.76</v>
+        <v>122.6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="B67">
-        <v>13.18</v>
+        <v>13.37</v>
       </c>
       <c r="C67">
-        <v>123.42</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
       <c r="B68">
-        <v>13.06</v>
+        <v>13.26</v>
       </c>
       <c r="C68">
-        <v>125.14</v>
+        <v>123.76</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>1.08</v>
+        <v>1.04</v>
       </c>
       <c r="B69">
-        <v>12.96</v>
+        <v>13.18</v>
       </c>
       <c r="C69">
-        <v>125.88</v>
+        <v>123.42</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="B70">
-        <v>12.86</v>
+        <v>13.06</v>
       </c>
       <c r="C70">
-        <v>126.67</v>
+        <v>125.14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="B71">
+        <v>12.96</v>
+      </c>
+      <c r="C71">
+        <v>125.88</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B73">
-        <v>13.3</v>
-      </c>
-      <c r="C73">
-        <v>121.66</v>
+      <c r="A72" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B72">
+        <v>12.86</v>
+      </c>
+      <c r="C72">
+        <v>126.67</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
-        <v>0.92</v>
-      </c>
-      <c r="B74">
-        <v>13.32</v>
-      </c>
-      <c r="C74">
-        <v>121.95</v>
+      <c r="A74" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="B75">
-        <v>13.33</v>
+        <v>13.3</v>
       </c>
       <c r="C75">
-        <v>122.25</v>
+        <v>121.66</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="B76">
-        <v>13.35</v>
+        <v>13.32</v>
       </c>
       <c r="C76">
-        <v>122.55</v>
+        <v>121.95</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="B77">
-        <v>13.36</v>
+        <v>13.33</v>
       </c>
       <c r="C77">
-        <v>122.85</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="B78">
-        <v>13.37</v>
+        <v>13.35</v>
       </c>
       <c r="C78">
-        <v>123.14</v>
+        <v>122.55</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="B79">
-        <v>13.39</v>
+        <v>13.36</v>
       </c>
       <c r="C79">
-        <v>123.44</v>
+        <v>122.85</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="B80">
-        <v>13.4</v>
+        <v>13.37</v>
       </c>
       <c r="C80">
-        <v>123.74</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
       <c r="B81">
-        <v>13.37</v>
+        <v>13.39</v>
       </c>
       <c r="C81">
-        <v>124.05</v>
+        <v>123.44</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>1.08</v>
+        <v>1.04</v>
       </c>
       <c r="B82">
-        <v>13.39</v>
+        <v>13.4</v>
       </c>
       <c r="C82">
-        <v>124.35</v>
+        <v>123.74</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="B83">
+        <v>13.37</v>
+      </c>
+      <c r="C83">
+        <v>124.05</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="B84">
+        <v>13.39</v>
+      </c>
+      <c r="C84">
+        <v>124.35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B83">
+      <c r="B85">
         <v>13.4</v>
       </c>
-      <c r="C83">
+      <c r="C85">
         <v>124.65</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
-        <v>-10</v>
-      </c>
-      <c r="B87">
-        <v>13.41</v>
-      </c>
-      <c r="C87">
-        <v>123.27</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <v>-8</v>
-      </c>
-      <c r="B88">
-        <v>13.4</v>
-      </c>
-      <c r="C88">
-        <v>123.24</v>
+      <c r="A88" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="B89">
-        <v>13.39</v>
+        <v>13.41</v>
       </c>
       <c r="C89">
-        <v>123.21</v>
+        <v>123.27</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>-4</v>
+        <v>-8</v>
       </c>
       <c r="B90">
-        <v>13.39</v>
+        <v>13.4</v>
       </c>
       <c r="C90">
-        <v>123.19</v>
+        <v>123.24</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="B91">
-        <v>13.38</v>
+        <v>13.39</v>
       </c>
       <c r="C91">
-        <v>123.16</v>
+        <v>123.21</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="B92">
-        <v>13.37</v>
+        <v>13.39</v>
       </c>
       <c r="C92">
-        <v>123.14</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B93">
-        <v>13.37</v>
+        <v>13.38</v>
       </c>
       <c r="C93">
-        <v>123.12</v>
+        <v>123.16</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B94">
-        <v>13.36</v>
+        <v>13.37</v>
       </c>
       <c r="C94">
-        <v>123.11</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B95">
-        <v>13.35</v>
+        <v>13.37</v>
       </c>
       <c r="C95">
-        <v>123.09</v>
+        <v>123.12</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B96">
-        <v>13.34</v>
+        <v>13.36</v>
       </c>
       <c r="C96">
-        <v>123.08</v>
+        <v>123.11</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B97">
-        <v>13.33</v>
+        <v>13.35</v>
       </c>
       <c r="C97">
-        <v>123.07</v>
+        <v>123.09</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>8</v>
+      </c>
+      <c r="B98">
+        <v>13.34</v>
+      </c>
+      <c r="C98">
+        <v>123.08</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>-10</v>
-      </c>
-      <c r="B100">
-        <v>13.38</v>
-      </c>
-      <c r="C100">
-        <v>123.29</v>
+      <c r="A99" s="2">
+        <v>10</v>
+      </c>
+      <c r="B99">
+        <v>13.33</v>
+      </c>
+      <c r="C99">
+        <v>123.07</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>-8</v>
-      </c>
-      <c r="B101">
-        <v>13.37</v>
-      </c>
-      <c r="C101">
-        <v>123.25</v>
+      <c r="A101" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="B102">
-        <v>13.36</v>
+        <v>13.38</v>
       </c>
       <c r="C102">
-        <v>123.22</v>
+        <v>123.29</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>-4</v>
+        <v>-8</v>
       </c>
       <c r="B103">
-        <v>13.39</v>
+        <v>13.37</v>
       </c>
       <c r="C103">
-        <v>123.19</v>
+        <v>123.25</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="B104">
-        <v>13.38</v>
+        <v>13.36</v>
       </c>
       <c r="C104">
-        <v>123.17</v>
+        <v>123.22</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="B105">
-        <v>13.37</v>
+        <v>13.39</v>
       </c>
       <c r="C105">
-        <v>123.14</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B106">
-        <v>13.37</v>
+        <v>13.38</v>
       </c>
       <c r="C106">
-        <v>123.13</v>
+        <v>123.17</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B107">
-        <v>13.36</v>
+        <v>13.37</v>
       </c>
       <c r="C107">
-        <v>123.11</v>
+        <v>123.14</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B108">
-        <v>13.35</v>
+        <v>13.37</v>
       </c>
       <c r="C108">
-        <v>123.09</v>
+        <v>123.13</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B109">
-        <v>13.35</v>
+        <v>13.36</v>
       </c>
       <c r="C109">
-        <v>123.08</v>
+        <v>123.11</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
+        <v>6</v>
+      </c>
+      <c r="B110">
+        <v>13.35</v>
+      </c>
+      <c r="C110">
+        <v>123.09</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>8</v>
+      </c>
+      <c r="B111">
+        <v>13.35</v>
+      </c>
+      <c r="C111">
+        <v>123.08</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112">
         <v>10</v>
       </c>
-      <c r="B110">
+      <c r="B112">
         <v>13.34</v>
       </c>
-      <c r="C110">
+      <c r="C112">
         <v>123.07</v>
       </c>
     </row>

</xml_diff>